<commit_message>
Budget creation has been updated
</commit_message>
<xml_diff>
--- a/Itokotons/input_data/Budgetcreation_TestData.xlsx
+++ b/Itokotons/input_data/Budgetcreation_TestData.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA8CBDC-C5BA-43AE-96E5-2ACBD2953DE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13635" windowHeight="6120"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BudgetCreationInputData" sheetId="4" r:id="rId1"/>
     <sheet name="Testcases" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="84">
   <si>
     <t>Username</t>
   </si>
@@ -269,23 +270,19 @@
     <t>Automation_Test_Approver_Remarks</t>
   </si>
   <si>
-    <t>BUD-20FH-0130</t>
-  </si>
-  <si>
-    <t>607099001-ACCRUED EXPENSES - ADVERTISING BY DEALERS</t>
-  </si>
-  <si>
-    <t>617001001-WARRANTY RESERVE</t>
-  </si>
-  <si>
     <t>BUD-20FH-0131</t>
+  </si>
+  <si>
+    <t>617392821-RANTY RESER</t>
+  </si>
+  <si>
+    <t>607092921-AED EXPENSES</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -419,6 +416,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -454,6 +468,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -629,26 +660,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="18.20703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="25.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="25.7109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="1" max="1" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="25.7109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -694,16 +725,16 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E2">
         <v>1000</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G2">
         <v>2000</v>
@@ -728,19 +759,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="5.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="52.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="26.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="52.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -999,17 +1030,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="22.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="30.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="34.7109375" collapsed="true"/>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="30.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="34.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>